<commit_message>
updated service and added customflow project
</commit_message>
<xml_diff>
--- a/customflows/src/main/resources/Sanity.xlsx
+++ b/customflows/src/main/resources/Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Automation_Project\customflows\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E8B3A0-8707-4805-9B18-7AEFCB9D295C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872A0E80-DCE1-42F7-AE99-12BA9A938DD3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>CFForm</t>
+  </si>
+  <si>
+    <t>TestData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -511,7 +514,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
modified custom flow tests with update logic
</commit_message>
<xml_diff>
--- a/customflows/src/main/resources/Sanity.xlsx
+++ b/customflows/src/main/resources/Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\Automation_Project\customflows\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872A0E80-DCE1-42F7-AE99-12BA9A938DD3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F9D79-AE19-4CE4-919C-964CF827CF3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -460,7 +460,7 @@
   <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -508,6 +508,9 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">

</xml_diff>